<commit_message>
Sequential removing edges - results
</commit_message>
<xml_diff>
--- a/figures/perf_experiments.xlsx
+++ b/figures/perf_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\partii\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F61486F-1283-4289-8622-0DF47DE7E9ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D18091B-83FA-48FD-9B79-AF1FEED7DE47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECB749D5-8467-4F35-AEC5-92A4EDA5AFC0}"/>
+    <workbookView xWindow="-120" yWindow="-13620" windowWidth="21840" windowHeight="13740" xr2:uid="{ECB749D5-8467-4F35-AEC5-92A4EDA5AFC0}"/>
   </bookViews>
   <sheets>
     <sheet name="experiments" sheetId="1" r:id="rId1"/>
@@ -493,22 +493,22 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G2">
-        <v>2282</v>
+        <v>2117</v>
       </c>
       <c r="H2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2">
-        <v>2316.5360000000001</v>
+        <v>2186.201</v>
       </c>
       <c r="J2">
-        <v>47798.319000000003</v>
+        <v>48462.919000000002</v>
       </c>
       <c r="K2">
-        <v>216.001</v>
+        <v>215.40899999999999</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -528,22 +528,22 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>149</v>
+        <v>54</v>
       </c>
       <c r="G3">
-        <v>2728</v>
+        <v>2218</v>
       </c>
       <c r="H3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3">
-        <v>2895.1350000000002</v>
+        <v>2289.8980000000001</v>
       </c>
       <c r="J3">
-        <v>81365.308999999994</v>
+        <v>52099.637999999999</v>
       </c>
       <c r="K3">
-        <v>282.73099999999999</v>
+        <v>207.739</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -563,22 +563,22 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="G4">
-        <v>27041</v>
+        <v>21342</v>
       </c>
       <c r="H4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I4">
-        <v>27163.304</v>
+        <v>21421.827000000001</v>
       </c>
       <c r="J4">
-        <v>824238.22699999996</v>
+        <v>535151.94099999999</v>
       </c>
       <c r="K4">
-        <v>1022.715</v>
+        <v>670.45399999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>